<commit_message>
HTML -> Introduction, Text, List, Links
</commit_message>
<xml_diff>
--- a/HTML_CSS_Responsive_Web_Design_Course.xlsx
+++ b/HTML_CSS_Responsive_Web_Design_Course.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7390" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7390"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="686">
   <si>
     <t>URL</t>
   </si>
@@ -2074,13 +2074,16 @@
   </si>
   <si>
     <t>An Introduction to CSS</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2119,8 +2122,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2148,6 +2159,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2274,7 +2291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2332,6 +2349,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2342,15 +2368,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2373,6 +2390,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3092,8 +3118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3113,7 +3139,7 @@
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="31"/>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="26" t="s">
         <v>683</v>
       </c>
     </row>
@@ -3130,16 +3156,16 @@
       <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
@@ -3150,13 +3176,13 @@
       <c r="D4" s="14">
         <v>9.2905092592592595E-2</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -3171,6 +3197,9 @@
       <c r="D6" s="21">
         <v>2.1296296296296298E-3</v>
       </c>
+      <c r="E6" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -3185,6 +3214,9 @@
       <c r="D7" s="21">
         <v>2.7546296296296294E-3</v>
       </c>
+      <c r="E7" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -3199,6 +3231,9 @@
       <c r="D8" s="21">
         <v>4.155092592592593E-3</v>
       </c>
+      <c r="E8" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -3213,6 +3248,9 @@
       <c r="D9" s="21">
         <v>2.2106481481481478E-3</v>
       </c>
+      <c r="E9" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -3227,6 +3265,9 @@
       <c r="D10" s="21">
         <v>5.1736111111111115E-3</v>
       </c>
+      <c r="E10" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -3241,6 +3282,9 @@
       <c r="D11" s="21">
         <v>2.1064814814814813E-3</v>
       </c>
+      <c r="E11" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -3255,6 +3299,9 @@
       <c r="D12" s="21">
         <v>1.5624999999999999E-3</v>
       </c>
+      <c r="E12" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
@@ -3269,12 +3316,15 @@
       <c r="D13" s="21">
         <v>8.6805555555555551E-4</v>
       </c>
+      <c r="E13" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="39"/>
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -3289,6 +3339,9 @@
       <c r="D15" s="21">
         <v>8.6805555555555551E-4</v>
       </c>
+      <c r="E15" s="37" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -3303,8 +3356,11 @@
       <c r="D16" s="21">
         <v>8.449074074074075E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E16" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -3317,8 +3373,11 @@
       <c r="D17" s="21">
         <v>1.2268518518518518E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E17" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
@@ -3331,8 +3390,11 @@
       <c r="D18" s="21">
         <v>1.6319444444444445E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E18" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
@@ -3345,8 +3407,11 @@
       <c r="D19" s="21">
         <v>3.6342592592592594E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E19" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>60</v>
       </c>
@@ -3359,8 +3424,11 @@
       <c r="D20" s="21">
         <v>2.3263888888888887E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E20" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>61</v>
       </c>
@@ -3373,8 +3441,11 @@
       <c r="D21" s="21">
         <v>4.8726851851851856E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E21" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
@@ -3387,8 +3458,11 @@
       <c r="D22" s="21">
         <v>2.2453703703703702E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E22" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -3401,8 +3475,11 @@
       <c r="D23" s="21">
         <v>4.5717592592592589E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E23" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -3415,14 +3492,17 @@
       <c r="D24" s="21">
         <v>6.3657407407407402E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
+      <c r="E24" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="28"/>
-    </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>63</v>
       </c>
@@ -3435,8 +3515,11 @@
       <c r="D26" s="21">
         <v>3.1250000000000001E-4</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E26" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
@@ -3449,8 +3532,11 @@
       <c r="D27" s="21">
         <v>8.1018518518518516E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E27" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
@@ -3463,8 +3549,11 @@
       <c r="D28" s="21">
         <v>4.0393518518518521E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E28" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
@@ -3477,8 +3566,11 @@
       <c r="D29" s="21">
         <v>3.5416666666666665E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E29" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
@@ -3491,14 +3583,17 @@
       <c r="D30" s="21">
         <v>4.2824074074074075E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="27" t="s">
+      <c r="E30" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="28"/>
-    </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="39"/>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
@@ -3511,8 +3606,11 @@
       <c r="D32" s="21">
         <v>4.6296296296296293E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E32" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>79</v>
       </c>
@@ -3525,8 +3623,11 @@
       <c r="D33" s="21">
         <v>2.5115740740740741E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E33" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>80</v>
       </c>
@@ -3539,8 +3640,11 @@
       <c r="D34" s="21">
         <v>2.8240740740740739E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E34" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>81</v>
       </c>
@@ -3553,8 +3657,11 @@
       <c r="D35" s="21">
         <v>4.8611111111111104E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E35" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>82</v>
       </c>
@@ -3567,8 +3674,11 @@
       <c r="D36" s="21">
         <v>4.0972222222222226E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E36" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>83</v>
       </c>
@@ -3581,8 +3691,11 @@
       <c r="D37" s="21">
         <v>6.134259259259259E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E37" s="37" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>94</v>
       </c>
@@ -3596,13 +3709,13 @@
         <v>4.0509259259259258E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="27" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="28"/>
-    </row>
-    <row r="40" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39" s="25"/>
+    </row>
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -3616,7 +3729,7 @@
         <v>7.291666666666667E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>98</v>
       </c>
@@ -3630,7 +3743,7 @@
         <v>1.1689814814814816E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>99</v>
       </c>
@@ -3644,7 +3757,7 @@
         <v>1.5740740740740741E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>100</v>
       </c>
@@ -3658,7 +3771,7 @@
         <v>3.1018518518518522E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>101</v>
       </c>
@@ -3672,7 +3785,7 @@
         <v>2.3611111111111111E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>102</v>
       </c>
@@ -3686,7 +3799,7 @@
         <v>2.2685185185185182E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>103</v>
       </c>
@@ -3700,7 +3813,7 @@
         <v>4.6180555555555558E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>104</v>
       </c>
@@ -3714,11 +3827,11 @@
         <v>4.0509259259259258E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="27" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="28"/>
+      <c r="B48" s="25"/>
     </row>
     <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
@@ -3791,12 +3904,12 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="7"/>
@@ -3809,10 +3922,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="28"/>
+      <c r="B57" s="25"/>
     </row>
     <row r="58" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
@@ -3941,10 +4054,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="B67" s="28"/>
+      <c r="B67" s="25"/>
     </row>
     <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
@@ -4101,10 +4214,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="27" t="s">
+      <c r="A79" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="B79" s="28"/>
+      <c r="B79" s="25"/>
     </row>
     <row r="80" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
@@ -4233,10 +4346,10 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="27" t="s">
+      <c r="A89" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="B89" s="28"/>
+      <c r="B89" s="25"/>
     </row>
     <row r="90" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
@@ -4337,10 +4450,10 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="27" t="s">
+      <c r="A97" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="B97" s="28"/>
+      <c r="B97" s="25"/>
     </row>
     <row r="98" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
@@ -4455,12 +4568,12 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="29" t="s">
+      <c r="A107" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="B107" s="29"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="29"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="12"/>
@@ -4473,10 +4586,10 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" s="27" t="s">
+      <c r="A109" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="B109" s="28"/>
+      <c r="B109" s="25"/>
     </row>
     <row r="110" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
@@ -4717,10 +4830,10 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="B127" s="28"/>
+      <c r="B127" s="25"/>
     </row>
     <row r="128" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
@@ -4849,10 +4962,10 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="27" t="s">
+      <c r="A137" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="B137" s="28"/>
+      <c r="B137" s="25"/>
     </row>
     <row r="138" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
@@ -4967,10 +5080,10 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A146" s="27" t="s">
+      <c r="A146" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="B146" s="28"/>
+      <c r="B146" s="25"/>
     </row>
     <row r="147" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
@@ -5043,12 +5156,12 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A153" s="29" t="s">
+      <c r="A153" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="B153" s="29"/>
-      <c r="C153" s="29"/>
-      <c r="D153" s="29"/>
+      <c r="B153" s="23"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="23"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="15"/>
@@ -5061,10 +5174,10 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A155" s="27" t="s">
+      <c r="A155" s="24" t="s">
         <v>458</v>
       </c>
-      <c r="B155" s="28"/>
+      <c r="B155" s="25"/>
     </row>
     <row r="156" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
@@ -5193,10 +5306,10 @@
       </c>
     </row>
     <row r="165" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="26" t="s">
+      <c r="A165" s="29" t="s">
         <v>483</v>
       </c>
-      <c r="B165" s="26"/>
+      <c r="B165" s="29"/>
     </row>
     <row r="166" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
@@ -5367,10 +5480,10 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A178" s="26" t="s">
+      <c r="A178" s="29" t="s">
         <v>519</v>
       </c>
-      <c r="B178" s="26"/>
+      <c r="B178" s="29"/>
     </row>
     <row r="179" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
@@ -5513,10 +5626,10 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A189" s="26" t="s">
+      <c r="A189" s="29" t="s">
         <v>547</v>
       </c>
-      <c r="B189" s="26"/>
+      <c r="B189" s="29"/>
     </row>
     <row r="190" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
@@ -5659,10 +5772,10 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A200" s="26" t="s">
+      <c r="A200" s="29" t="s">
         <v>577</v>
       </c>
-      <c r="B200" s="26"/>
+      <c r="B200" s="29"/>
     </row>
     <row r="201" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="3" t="s">
@@ -5777,10 +5890,10 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A209" s="26" t="s">
+      <c r="A209" s="29" t="s">
         <v>619</v>
       </c>
-      <c r="B209" s="26"/>
+      <c r="B209" s="29"/>
     </row>
     <row r="210" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A210" s="3" t="s">
@@ -5881,10 +5994,10 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A217" s="26" t="s">
+      <c r="A217" s="29" t="s">
         <v>618</v>
       </c>
-      <c r="B217" s="26"/>
+      <c r="B217" s="29"/>
     </row>
     <row r="218" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="3" t="s">
@@ -5999,10 +6112,10 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A226" s="26" t="s">
+      <c r="A226" s="29" t="s">
         <v>642</v>
       </c>
-      <c r="B226" s="26"/>
+      <c r="B226" s="29"/>
     </row>
     <row r="227" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A227" s="3" t="s">
@@ -6104,19 +6217,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A48:B48"/>
     <mergeCell ref="E1:E4"/>
     <mergeCell ref="A217:B217"/>
     <mergeCell ref="A226:B226"/>
@@ -6133,6 +6233,19 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1"/>
@@ -6342,7 +6455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>